<commit_message>
Add comprehensive Requirement/User Story/Goal Mapper for Agile coaching
</commit_message>
<xml_diff>
--- a/RPG/images/U4 and 5 Image data.xlsx
+++ b/RPG/images/U4 and 5 Image data.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tedtschopp/Documents/GitHub/tedt.org/RPG/images/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tedtschopp/Developer/tedt.org/RPG/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2DBAF3E2-3097-2F4E-8955-5FD200CCD821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23F17E2-3A1A-4D42-9C58-41660B51FD22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31640" yWindow="500" windowWidth="28060" windowHeight="17460" xr2:uid="{899837AF-DA2E-EC45-BB45-3151DAABF807}"/>
+    <workbookView xWindow="25600" yWindow="620" windowWidth="25620" windowHeight="28180" xr2:uid="{899837AF-DA2E-EC45-BB45-3151DAABF807}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,30 +36,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1192" uniqueCount="917">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1205" uniqueCount="927">
   <si>
     <t>Offset</t>
   </si>
@@ -2713,9 +2691,6 @@
     <t>Fence - E-W</t>
   </si>
   <si>
-    <t>More Bat?</t>
-  </si>
-  <si>
     <t>NW</t>
   </si>
   <si>
@@ -2810,6 +2785,39 @@
   </si>
   <si>
     <t>8 stones</t>
+  </si>
+  <si>
+    <t>Procolmation</t>
+  </si>
+  <si>
+    <t>a grandfather clock, Tick</t>
+  </si>
+  <si>
+    <t>a grandfather clock, Tock</t>
+  </si>
+  <si>
+    <t>Fire Flicker for Torch left</t>
+  </si>
+  <si>
+    <t>Fire Flicker for Torch Right</t>
+  </si>
+  <si>
+    <t>Fire Flicker for Brazer</t>
+  </si>
+  <si>
+    <t>Fireflicker for Cooking Spit</t>
+  </si>
+  <si>
+    <t>Fire Flicker for Fireplace</t>
+  </si>
+  <si>
+    <t>Fire Flicker for Lampost</t>
+  </si>
+  <si>
+    <t>Fire Flicker for Candles</t>
+  </si>
+  <si>
+    <t>Fire Flicker for Stove</t>
   </si>
 </sst>
 </file>
@@ -2870,11 +2878,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -2899,15 +2906,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1943100</xdr:colOff>
-      <xdr:row>184</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>203</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>216</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>235</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2937,7 +2944,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5753100" y="37490400"/>
+          <a:off x="4508500" y="41440100"/>
           <a:ext cx="13004800" cy="6502400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3277,16 +3284,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C257557-0CE3-7C44-B9BE-3642D5280C90}">
-  <dimension ref="A1:E337"/>
+  <dimension ref="A1:E522"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B274" workbookViewId="0">
-      <selection activeCell="E263" sqref="E263"/>
+    <sheetView tabSelected="1" topLeftCell="B196" workbookViewId="0">
+      <selection activeCell="D208" sqref="D208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="3"/>
-    <col min="3" max="3" width="28.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3328,7 +3334,7 @@
       <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>682</v>
       </c>
     </row>
@@ -3342,7 +3348,7 @@
       <c r="D4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>683</v>
       </c>
     </row>
@@ -3359,7 +3365,7 @@
       <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>684</v>
       </c>
     </row>
@@ -3376,7 +3382,7 @@
       <c r="D6" s="2" t="s">
         <v>517</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>685</v>
       </c>
     </row>
@@ -3393,7 +3399,7 @@
       <c r="D7" s="2" t="s">
         <v>518</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>686</v>
       </c>
     </row>
@@ -3410,7 +3416,7 @@
       <c r="D8" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>687</v>
       </c>
     </row>
@@ -3427,7 +3433,7 @@
       <c r="D9" s="2" t="s">
         <v>520</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>688</v>
       </c>
     </row>
@@ -3444,7 +3450,7 @@
       <c r="D10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="4" t="s">
         <v>687</v>
       </c>
     </row>
@@ -3461,7 +3467,7 @@
       <c r="D11" s="2" t="s">
         <v>521</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="4" t="s">
         <v>689</v>
       </c>
     </row>
@@ -3478,7 +3484,7 @@
       <c r="D12" s="2" t="s">
         <v>522</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="4" t="s">
         <v>690</v>
       </c>
     </row>
@@ -3495,7 +3501,7 @@
       <c r="D13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="4" t="s">
         <v>691</v>
       </c>
     </row>
@@ -3512,7 +3518,7 @@
       <c r="D14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="4" t="s">
         <v>692</v>
       </c>
     </row>
@@ -3529,7 +3535,7 @@
       <c r="D15" s="2" t="s">
         <v>523</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="4" t="s">
         <v>693</v>
       </c>
     </row>
@@ -3574,7 +3580,7 @@
       <c r="D18" s="2" t="s">
         <v>526</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="4" t="s">
         <v>694</v>
       </c>
     </row>
@@ -3591,7 +3597,7 @@
       <c r="D19" s="2" t="s">
         <v>527</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="4" t="s">
         <v>695</v>
       </c>
     </row>
@@ -3608,7 +3614,7 @@
       <c r="D20" s="2" t="s">
         <v>528</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="4" t="s">
         <v>696</v>
       </c>
     </row>
@@ -3625,7 +3631,7 @@
       <c r="D21" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="4" t="s">
         <v>697</v>
       </c>
     </row>
@@ -3642,7 +3648,7 @@
       <c r="D22" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="4" t="s">
         <v>698</v>
       </c>
     </row>
@@ -3659,7 +3665,7 @@
       <c r="D23" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="4" t="s">
         <v>699</v>
       </c>
     </row>
@@ -3676,7 +3682,7 @@
       <c r="D24" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E24" s="4" t="s">
         <v>700</v>
       </c>
     </row>
@@ -3693,7 +3699,7 @@
       <c r="D25" s="2" t="s">
         <v>530</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="E25" s="4" t="s">
         <v>701</v>
       </c>
     </row>
@@ -3710,7 +3716,7 @@
       <c r="D26" s="2" t="s">
         <v>531</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E26" s="4" t="s">
         <v>702</v>
       </c>
     </row>
@@ -3727,7 +3733,7 @@
       <c r="D27" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="E27" s="4" t="s">
         <v>703</v>
       </c>
     </row>
@@ -3744,7 +3750,7 @@
       <c r="D28" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="E28" s="4" t="s">
         <v>704</v>
       </c>
     </row>
@@ -3761,7 +3767,7 @@
       <c r="D29" s="2" t="s">
         <v>533</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="E29" s="4" t="s">
         <v>705</v>
       </c>
     </row>
@@ -3792,7 +3798,7 @@
       <c r="D31" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="E31" s="4" t="s">
         <v>706</v>
       </c>
     </row>
@@ -3837,7 +3843,7 @@
       <c r="D34" s="2" t="s">
         <v>537</v>
       </c>
-      <c r="E34" s="5" t="s">
+      <c r="E34" s="4" t="s">
         <v>707</v>
       </c>
     </row>
@@ -3907,9 +3913,9 @@
       <c r="C39" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D39" t="e" cm="1">
-        <f t="array" ref="D39">+ Path</f>
-        <v>#NAME?</v>
+      <c r="D39" s="2" t="str">
+        <f>"+ Path"</f>
+        <v>+ Path</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -3925,7 +3931,7 @@
       <c r="D40" s="2" t="s">
         <v>542</v>
       </c>
-      <c r="E40" s="5" t="s">
+      <c r="E40" s="4" t="s">
         <v>708</v>
       </c>
     </row>
@@ -3956,7 +3962,7 @@
       <c r="D42" s="2" t="s">
         <v>544</v>
       </c>
-      <c r="E42" s="5" t="s">
+      <c r="E42" s="4" t="s">
         <v>709</v>
       </c>
     </row>
@@ -3973,7 +3979,7 @@
       <c r="D43" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="E43" s="5" t="s">
+      <c r="E43" s="4" t="s">
         <v>710</v>
       </c>
     </row>
@@ -3990,7 +3996,7 @@
       <c r="D44" s="2" t="s">
         <v>546</v>
       </c>
-      <c r="E44" s="5" t="s">
+      <c r="E44" s="4" t="s">
         <v>711</v>
       </c>
     </row>
@@ -4007,7 +4013,7 @@
       <c r="D45" s="2" t="s">
         <v>547</v>
       </c>
-      <c r="E45" s="5" t="s">
+      <c r="E45" s="4" t="s">
         <v>712</v>
       </c>
     </row>
@@ -4024,7 +4030,7 @@
       <c r="D46" s="2" t="s">
         <v>548</v>
       </c>
-      <c r="E46" s="5" t="s">
+      <c r="E46" s="4" t="s">
         <v>713</v>
       </c>
     </row>
@@ -4041,7 +4047,7 @@
       <c r="D47" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="E47" s="5" t="s">
+      <c r="E47" s="4" t="s">
         <v>714</v>
       </c>
     </row>
@@ -4058,7 +4064,7 @@
       <c r="D48" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="E48" s="5" t="s">
+      <c r="E48" s="4" t="s">
         <v>715</v>
       </c>
     </row>
@@ -4187,7 +4193,7 @@
       <c r="D57" s="2" t="s">
         <v>559</v>
       </c>
-      <c r="E57" s="5" t="s">
+      <c r="E57" s="4" t="s">
         <v>716</v>
       </c>
     </row>
@@ -4302,7 +4308,7 @@
       <c r="D65" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="E65" s="5" t="s">
+      <c r="E65" s="4" t="s">
         <v>717</v>
       </c>
     </row>
@@ -4319,7 +4325,7 @@
       <c r="D66" s="2" t="s">
         <v>566</v>
       </c>
-      <c r="E66" s="5" t="s">
+      <c r="E66" s="4" t="s">
         <v>718</v>
       </c>
     </row>
@@ -4336,7 +4342,7 @@
       <c r="D67" s="2" t="s">
         <v>570</v>
       </c>
-      <c r="E67" s="5" t="s">
+      <c r="E67" s="4" t="s">
         <v>719</v>
       </c>
     </row>
@@ -4395,7 +4401,7 @@
       <c r="D71" s="2" t="s">
         <v>569</v>
       </c>
-      <c r="E71" s="5" t="s">
+      <c r="E71" s="4" t="s">
         <v>720</v>
       </c>
     </row>
@@ -4412,7 +4418,7 @@
       <c r="D72" s="2" t="s">
         <v>571</v>
       </c>
-      <c r="E72" s="5" t="s">
+      <c r="E72" s="4" t="s">
         <v>721</v>
       </c>
     </row>
@@ -4429,7 +4435,7 @@
       <c r="D73" s="2" t="s">
         <v>573</v>
       </c>
-      <c r="E73" s="5" t="s">
+      <c r="E73" s="4" t="s">
         <v>722</v>
       </c>
     </row>
@@ -4446,7 +4452,7 @@
       <c r="D74" s="2" t="s">
         <v>573</v>
       </c>
-      <c r="E74" s="5" t="s">
+      <c r="E74" s="4" t="s">
         <v>723</v>
       </c>
     </row>
@@ -4463,7 +4469,7 @@
       <c r="D75" s="2" t="s">
         <v>574</v>
       </c>
-      <c r="E75" s="5" t="s">
+      <c r="E75" s="4" t="s">
         <v>724</v>
       </c>
     </row>
@@ -4480,7 +4486,7 @@
       <c r="D76" s="2" t="s">
         <v>575</v>
       </c>
-      <c r="E76" s="5" t="s">
+      <c r="E76" s="4" t="s">
         <v>725</v>
       </c>
     </row>
@@ -4497,7 +4503,7 @@
       <c r="D77" s="2" t="s">
         <v>576</v>
       </c>
-      <c r="E77" s="5" t="s">
+      <c r="E77" s="4" t="s">
         <v>726</v>
       </c>
     </row>
@@ -4514,7 +4520,7 @@
       <c r="D78" s="2" t="s">
         <v>577</v>
       </c>
-      <c r="E78" s="5" t="s">
+      <c r="E78" s="4" t="s">
         <v>727</v>
       </c>
     </row>
@@ -4531,7 +4537,7 @@
       <c r="D79" s="2" t="s">
         <v>579</v>
       </c>
-      <c r="E79" s="5" t="s">
+      <c r="E79" s="4" t="s">
         <v>728</v>
       </c>
     </row>
@@ -4548,7 +4554,7 @@
       <c r="D80" s="2" t="s">
         <v>578</v>
       </c>
-      <c r="E80" s="5" t="s">
+      <c r="E80" s="4" t="s">
         <v>729</v>
       </c>
     </row>
@@ -4565,7 +4571,7 @@
       <c r="D81" s="2" t="s">
         <v>580</v>
       </c>
-      <c r="E81" s="5" t="s">
+      <c r="E81" s="4" t="s">
         <v>730</v>
       </c>
     </row>
@@ -4582,7 +4588,7 @@
       <c r="D82" s="2" t="s">
         <v>580</v>
       </c>
-      <c r="E82" s="5" t="s">
+      <c r="E82" s="4" t="s">
         <v>730</v>
       </c>
     </row>
@@ -4599,7 +4605,7 @@
       <c r="D83" s="2" t="s">
         <v>580</v>
       </c>
-      <c r="E83" s="5" t="s">
+      <c r="E83" s="4" t="s">
         <v>730</v>
       </c>
     </row>
@@ -4616,7 +4622,7 @@
       <c r="D84" s="2" t="s">
         <v>580</v>
       </c>
-      <c r="E84" s="5" t="s">
+      <c r="E84" s="4" t="s">
         <v>730</v>
       </c>
     </row>
@@ -4633,7 +4639,7 @@
       <c r="D85" s="2" t="s">
         <v>580</v>
       </c>
-      <c r="E85" s="5" t="s">
+      <c r="E85" s="4" t="s">
         <v>730</v>
       </c>
     </row>
@@ -4650,7 +4656,7 @@
       <c r="D86" s="2" t="s">
         <v>580</v>
       </c>
-      <c r="E86" s="5" t="s">
+      <c r="E86" s="4" t="s">
         <v>730</v>
       </c>
     </row>
@@ -4667,7 +4673,7 @@
       <c r="D87" s="2" t="s">
         <v>580</v>
       </c>
-      <c r="E87" s="5" t="s">
+      <c r="E87" s="4" t="s">
         <v>730</v>
       </c>
     </row>
@@ -4684,7 +4690,7 @@
       <c r="D88" s="2" t="s">
         <v>580</v>
       </c>
-      <c r="E88" s="5" t="s">
+      <c r="E88" s="4" t="s">
         <v>730</v>
       </c>
     </row>
@@ -4701,7 +4707,7 @@
       <c r="D89" s="2" t="s">
         <v>581</v>
       </c>
-      <c r="E89" s="5" t="s">
+      <c r="E89" s="4" t="s">
         <v>731</v>
       </c>
     </row>
@@ -4718,7 +4724,7 @@
       <c r="D90" s="2" t="s">
         <v>582</v>
       </c>
-      <c r="E90" s="5" t="s">
+      <c r="E90" s="4" t="s">
         <v>732</v>
       </c>
     </row>
@@ -4735,7 +4741,7 @@
       <c r="D91" s="2" t="s">
         <v>583</v>
       </c>
-      <c r="E91" s="5" t="s">
+      <c r="E91" s="4" t="s">
         <v>733</v>
       </c>
     </row>
@@ -4752,7 +4758,7 @@
       <c r="D92" s="2" t="s">
         <v>584</v>
       </c>
-      <c r="E92" s="5" t="s">
+      <c r="E92" s="4" t="s">
         <v>734</v>
       </c>
     </row>
@@ -4769,7 +4775,7 @@
       <c r="D93" s="2" t="s">
         <v>585</v>
       </c>
-      <c r="E93" s="5" t="s">
+      <c r="E93" s="4" t="s">
         <v>735</v>
       </c>
     </row>
@@ -4786,7 +4792,7 @@
       <c r="D94" s="2" t="s">
         <v>586</v>
       </c>
-      <c r="E94" s="5" t="s">
+      <c r="E94" s="4" t="s">
         <v>735</v>
       </c>
     </row>
@@ -4803,7 +4809,7 @@
       <c r="D95" s="2" t="s">
         <v>587</v>
       </c>
-      <c r="E95" s="5" t="s">
+      <c r="E95" s="4" t="s">
         <v>736</v>
       </c>
     </row>
@@ -4820,7 +4826,7 @@
       <c r="D96" s="2" t="s">
         <v>588</v>
       </c>
-      <c r="E96" s="5" t="s">
+      <c r="E96" s="4" t="s">
         <v>736</v>
       </c>
     </row>
@@ -4837,7 +4843,7 @@
       <c r="D97" s="2" t="s">
         <v>589</v>
       </c>
-      <c r="E97" s="5" t="s">
+      <c r="E97" s="4" t="s">
         <v>737</v>
       </c>
     </row>
@@ -4854,7 +4860,7 @@
       <c r="D98" s="2" t="s">
         <v>590</v>
       </c>
-      <c r="E98" s="5" t="s">
+      <c r="E98" s="4" t="s">
         <v>737</v>
       </c>
     </row>
@@ -5277,7 +5283,7 @@
       <c r="D128" s="2" t="s">
         <v>618</v>
       </c>
-      <c r="E128" s="5" t="s">
+      <c r="E128" s="4" t="s">
         <v>738</v>
       </c>
     </row>
@@ -5294,7 +5300,7 @@
       <c r="D129" s="2" t="s">
         <v>621</v>
       </c>
-      <c r="E129" s="5" t="s">
+      <c r="E129" s="4" t="s">
         <v>739</v>
       </c>
     </row>
@@ -5353,7 +5359,7 @@
       <c r="D133" s="2" t="s">
         <v>625</v>
       </c>
-      <c r="E133" s="5" t="s">
+      <c r="E133" s="4" t="s">
         <v>740</v>
       </c>
     </row>
@@ -5370,7 +5376,7 @@
       <c r="D134" s="2" t="s">
         <v>626</v>
       </c>
-      <c r="E134" s="5" t="s">
+      <c r="E134" s="4" t="s">
         <v>741</v>
       </c>
     </row>
@@ -5387,7 +5393,7 @@
       <c r="D135" s="2" t="s">
         <v>627</v>
       </c>
-      <c r="E135" s="5" t="s">
+      <c r="E135" s="4" t="s">
         <v>742</v>
       </c>
     </row>
@@ -5404,7 +5410,7 @@
       <c r="D136" s="2" t="s">
         <v>628</v>
       </c>
-      <c r="E136" s="5" t="s">
+      <c r="E136" s="4" t="s">
         <v>743</v>
       </c>
     </row>
@@ -5421,7 +5427,7 @@
       <c r="D137" s="2" t="s">
         <v>629</v>
       </c>
-      <c r="E137" s="5" t="s">
+      <c r="E137" s="4" t="s">
         <v>744</v>
       </c>
     </row>
@@ -5438,7 +5444,7 @@
       <c r="D138" s="2" t="s">
         <v>630</v>
       </c>
-      <c r="E138" s="5" t="s">
+      <c r="E138" s="4" t="s">
         <v>732</v>
       </c>
     </row>
@@ -5469,7 +5475,7 @@
       <c r="D140" s="2" t="s">
         <v>632</v>
       </c>
-      <c r="E140" s="5" t="s">
+      <c r="E140" s="4" t="s">
         <v>745</v>
       </c>
     </row>
@@ -5486,7 +5492,7 @@
       <c r="D141" s="2" t="s">
         <v>633</v>
       </c>
-      <c r="E141" s="5" t="s">
+      <c r="E141" s="4" t="s">
         <v>746</v>
       </c>
     </row>
@@ -5503,7 +5509,7 @@
       <c r="D142" s="2" t="s">
         <v>634</v>
       </c>
-      <c r="E142" s="5" t="s">
+      <c r="E142" s="4" t="s">
         <v>747</v>
       </c>
     </row>
@@ -5520,7 +5526,7 @@
       <c r="D143" s="2" t="s">
         <v>635</v>
       </c>
-      <c r="E143" s="5" t="s">
+      <c r="E143" s="4" t="s">
         <v>748</v>
       </c>
     </row>
@@ -5537,7 +5543,7 @@
       <c r="D144" s="2" t="s">
         <v>636</v>
       </c>
-      <c r="E144" s="5" t="s">
+      <c r="E144" s="4" t="s">
         <v>749</v>
       </c>
     </row>
@@ -5596,7 +5602,7 @@
       <c r="D148" s="2" t="s">
         <v>640</v>
       </c>
-      <c r="E148" s="5" t="s">
+      <c r="E148" s="4" t="s">
         <v>750</v>
       </c>
     </row>
@@ -5613,7 +5619,7 @@
       <c r="D149" s="2" t="s">
         <v>641</v>
       </c>
-      <c r="E149" s="5" t="s">
+      <c r="E149" s="4" t="s">
         <v>751</v>
       </c>
     </row>
@@ -5644,7 +5650,7 @@
       <c r="D151" s="2" t="s">
         <v>672</v>
       </c>
-      <c r="E151" s="5" t="s">
+      <c r="E151" s="4" t="s">
         <v>752</v>
       </c>
     </row>
@@ -5675,7 +5681,7 @@
       <c r="D153" s="2" t="s">
         <v>643</v>
       </c>
-      <c r="E153" s="5" t="s">
+      <c r="E153" s="4" t="s">
         <v>753</v>
       </c>
     </row>
@@ -5692,7 +5698,7 @@
       <c r="D154" s="2" t="s">
         <v>644</v>
       </c>
-      <c r="E154" s="5" t="s">
+      <c r="E154" s="4" t="s">
         <v>754</v>
       </c>
     </row>
@@ -5737,7 +5743,7 @@
       <c r="D157" s="2" t="s">
         <v>647</v>
       </c>
-      <c r="E157" s="5" t="s">
+      <c r="E157" s="4" t="s">
         <v>755</v>
       </c>
     </row>
@@ -5754,7 +5760,7 @@
       <c r="D158" s="2" t="s">
         <v>648</v>
       </c>
-      <c r="E158" s="5" t="s">
+      <c r="E158" s="4" t="s">
         <v>756</v>
       </c>
     </row>
@@ -5771,7 +5777,7 @@
       <c r="D159" s="2" t="s">
         <v>649</v>
       </c>
-      <c r="E159" s="5" t="s">
+      <c r="E159" s="4" t="s">
         <v>757</v>
       </c>
     </row>
@@ -5788,7 +5794,7 @@
       <c r="D160" s="2" t="s">
         <v>650</v>
       </c>
-      <c r="E160" s="5" t="s">
+      <c r="E160" s="4" t="s">
         <v>732</v>
       </c>
     </row>
@@ -5805,7 +5811,7 @@
       <c r="D161" s="2" t="s">
         <v>651</v>
       </c>
-      <c r="E161" s="5" t="s">
+      <c r="E161" s="4" t="s">
         <v>758</v>
       </c>
     </row>
@@ -5819,10 +5825,10 @@
       <c r="C162" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="D162" s="5" t="s">
+      <c r="D162" s="4" t="s">
         <v>759</v>
       </c>
-      <c r="E162" s="5" t="s">
+      <c r="E162" s="4" t="s">
         <v>759</v>
       </c>
     </row>
@@ -5839,7 +5845,7 @@
       <c r="D163" s="2" t="s">
         <v>652</v>
       </c>
-      <c r="E163" s="5" t="s">
+      <c r="E163" s="4" t="s">
         <v>760</v>
       </c>
     </row>
@@ -5856,7 +5862,7 @@
       <c r="D164" s="2" t="s">
         <v>653</v>
       </c>
-      <c r="E164" s="5" t="s">
+      <c r="E164" s="4" t="s">
         <v>732</v>
       </c>
     </row>
@@ -5873,7 +5879,7 @@
       <c r="D165" s="2" t="s">
         <v>654</v>
       </c>
-      <c r="E165" s="5" t="s">
+      <c r="E165" s="4" t="s">
         <v>761</v>
       </c>
     </row>
@@ -5890,7 +5896,7 @@
       <c r="D166" s="2" t="s">
         <v>655</v>
       </c>
-      <c r="E166" s="5" t="s">
+      <c r="E166" s="4" t="s">
         <v>762</v>
       </c>
     </row>
@@ -5907,7 +5913,7 @@
       <c r="D167" s="2" t="s">
         <v>656</v>
       </c>
-      <c r="E167" s="5" t="s">
+      <c r="E167" s="4" t="s">
         <v>763</v>
       </c>
     </row>
@@ -5924,7 +5930,7 @@
       <c r="D168" s="2" t="s">
         <v>657</v>
       </c>
-      <c r="E168" s="5" t="s">
+      <c r="E168" s="4" t="s">
         <v>764</v>
       </c>
     </row>
@@ -5941,7 +5947,7 @@
       <c r="D169" s="2" t="s">
         <v>658</v>
       </c>
-      <c r="E169" s="5" t="s">
+      <c r="E169" s="4" t="s">
         <v>765</v>
       </c>
     </row>
@@ -5958,7 +5964,7 @@
       <c r="D170" s="2" t="s">
         <v>659</v>
       </c>
-      <c r="E170" s="5" t="s">
+      <c r="E170" s="4" t="s">
         <v>766</v>
       </c>
     </row>
@@ -5975,7 +5981,7 @@
       <c r="D171" s="2" t="s">
         <v>660</v>
       </c>
-      <c r="E171" s="5" t="s">
+      <c r="E171" s="4" t="s">
         <v>767</v>
       </c>
     </row>
@@ -6006,7 +6012,7 @@
       <c r="D173" s="2" t="s">
         <v>662</v>
       </c>
-      <c r="E173" s="5" t="s">
+      <c r="E173" s="4" t="s">
         <v>768</v>
       </c>
     </row>
@@ -6023,7 +6029,7 @@
       <c r="D174" s="2" t="s">
         <v>654</v>
       </c>
-      <c r="E174" s="5" t="s">
+      <c r="E174" s="4" t="s">
         <v>769</v>
       </c>
     </row>
@@ -6040,7 +6046,7 @@
       <c r="D175" s="2" t="s">
         <v>663</v>
       </c>
-      <c r="E175" s="5" t="s">
+      <c r="E175" s="4" t="s">
         <v>770</v>
       </c>
     </row>
@@ -6057,7 +6063,7 @@
       <c r="D176" s="2" t="s">
         <v>664</v>
       </c>
-      <c r="E176" s="5" t="s">
+      <c r="E176" s="4" t="s">
         <v>771</v>
       </c>
     </row>
@@ -6088,7 +6094,7 @@
       <c r="D178" s="2" t="s">
         <v>666</v>
       </c>
-      <c r="E178" s="5" t="s">
+      <c r="E178" s="4" t="s">
         <v>772</v>
       </c>
     </row>
@@ -6105,7 +6111,7 @@
       <c r="D179" s="2" t="s">
         <v>667</v>
       </c>
-      <c r="E179" s="5" t="s">
+      <c r="E179" s="4" t="s">
         <v>773</v>
       </c>
     </row>
@@ -6164,7 +6170,7 @@
       <c r="D183" s="2" t="s">
         <v>671</v>
       </c>
-      <c r="E183" s="5" t="s">
+      <c r="E183" s="4" t="s">
         <v>774</v>
       </c>
     </row>
@@ -6181,7 +6187,7 @@
       <c r="D184" s="2" t="s">
         <v>674</v>
       </c>
-      <c r="E184" s="5" t="s">
+      <c r="E184" s="4" t="s">
         <v>775</v>
       </c>
     </row>
@@ -6198,7 +6204,7 @@
       <c r="D185" s="2" t="s">
         <v>675</v>
       </c>
-      <c r="E185" s="5" t="s">
+      <c r="E185" s="4" t="s">
         <v>776</v>
       </c>
     </row>
@@ -6215,7 +6221,7 @@
       <c r="D186" s="2" t="s">
         <v>676</v>
       </c>
-      <c r="E186" s="5" t="s">
+      <c r="E186" s="4" t="s">
         <v>777</v>
       </c>
     </row>
@@ -6232,7 +6238,7 @@
       <c r="D187" s="2" t="s">
         <v>677</v>
       </c>
-      <c r="E187" s="5" t="s">
+      <c r="E187" s="4" t="s">
         <v>778</v>
       </c>
     </row>
@@ -6249,7 +6255,7 @@
       <c r="D188" s="2" t="s">
         <v>678</v>
       </c>
-      <c r="E188" s="5" t="s">
+      <c r="E188" s="4" t="s">
         <v>779</v>
       </c>
     </row>
@@ -6266,7 +6272,7 @@
       <c r="D189" s="2" t="s">
         <v>679</v>
       </c>
-      <c r="E189" s="5" t="s">
+      <c r="E189" s="4" t="s">
         <v>780</v>
       </c>
     </row>
@@ -6283,7 +6289,7 @@
       <c r="D190" s="2" t="s">
         <v>680</v>
       </c>
-      <c r="E190" s="5" t="s">
+      <c r="E190" s="4" t="s">
         <v>781</v>
       </c>
     </row>
@@ -6300,7 +6306,7 @@
       <c r="D191" s="2" t="s">
         <v>681</v>
       </c>
-      <c r="E191" s="5" t="s">
+      <c r="E191" s="4" t="s">
         <v>782</v>
       </c>
     </row>
@@ -6315,7 +6321,7 @@
         <v>383</v>
       </c>
       <c r="D192" s="2" t="s">
-        <v>299</v>
+        <v>919</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.2">
@@ -6329,7 +6335,7 @@
         <v>385</v>
       </c>
       <c r="D193" s="2" t="s">
-        <v>301</v>
+        <v>920</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
@@ -6343,7 +6349,7 @@
         <v>387</v>
       </c>
       <c r="D194" s="2" t="s">
-        <v>303</v>
+        <v>921</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.2">
@@ -6357,9 +6363,9 @@
         <v>389</v>
       </c>
       <c r="D195" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="E195" s="5" t="s">
+        <v>922</v>
+      </c>
+      <c r="E195" s="4" t="s">
         <v>732</v>
       </c>
     </row>
@@ -6418,7 +6424,7 @@
       <c r="D199" s="2" t="s">
         <v>880</v>
       </c>
-      <c r="E199" s="5" t="s">
+      <c r="E199" s="4" t="s">
         <v>783</v>
       </c>
     </row>
@@ -6435,7 +6441,7 @@
       <c r="D200" s="2" t="s">
         <v>881</v>
       </c>
-      <c r="E200" s="5" t="s">
+      <c r="E200" s="4" t="s">
         <v>784</v>
       </c>
     </row>
@@ -6466,7 +6472,7 @@
       <c r="D202" s="2" t="s">
         <v>883</v>
       </c>
-      <c r="E202" s="5" t="s">
+      <c r="E202" s="4" t="s">
         <v>785</v>
       </c>
     </row>
@@ -6483,7 +6489,7 @@
       <c r="D203" s="2" t="s">
         <v>882</v>
       </c>
-      <c r="E203" s="5" t="s">
+      <c r="E203" s="4" t="s">
         <v>732</v>
       </c>
     </row>
@@ -6498,7 +6504,7 @@
         <v>407</v>
       </c>
       <c r="D204" s="2" t="s">
-        <v>884</v>
+        <v>923</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.2">
@@ -6512,7 +6518,7 @@
         <v>409</v>
       </c>
       <c r="D205" s="2" t="s">
-        <v>884</v>
+        <v>924</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.2">
@@ -6526,7 +6532,7 @@
         <v>411</v>
       </c>
       <c r="D206" s="2" t="s">
-        <v>884</v>
+        <v>925</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.2">
@@ -6540,7 +6546,7 @@
         <v>413</v>
       </c>
       <c r="D207" s="2" t="s">
-        <v>884</v>
+        <v>926</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.2">
@@ -6554,7 +6560,7 @@
         <v>415</v>
       </c>
       <c r="D208" s="2" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.2">
@@ -6568,7 +6574,7 @@
         <v>417</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.2">
@@ -6582,7 +6588,7 @@
         <v>419</v>
       </c>
       <c r="D210" s="2" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.2">
@@ -6596,7 +6602,7 @@
         <v>421</v>
       </c>
       <c r="D211" s="2" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.2">
@@ -6610,9 +6616,9 @@
         <v>423</v>
       </c>
       <c r="D212" s="2" t="s">
-        <v>889</v>
-      </c>
-      <c r="E212" s="5" t="s">
+        <v>888</v>
+      </c>
+      <c r="E212" s="4" t="s">
         <v>786</v>
       </c>
     </row>
@@ -6627,9 +6633,9 @@
         <v>425</v>
       </c>
       <c r="D213" s="2" t="s">
-        <v>890</v>
-      </c>
-      <c r="E213" s="5" t="s">
+        <v>889</v>
+      </c>
+      <c r="E213" s="4" t="s">
         <v>732</v>
       </c>
     </row>
@@ -6644,7 +6650,7 @@
         <v>427</v>
       </c>
       <c r="D214" s="2" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.2">
@@ -6658,7 +6664,7 @@
         <v>429</v>
       </c>
       <c r="D215" s="2" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.2">
@@ -6672,7 +6678,7 @@
         <v>431</v>
       </c>
       <c r="D216" s="2" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.2">
@@ -6686,7 +6692,7 @@
         <v>433</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.2">
@@ -6700,7 +6706,7 @@
         <v>435</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.2">
@@ -6714,7 +6720,7 @@
         <v>437</v>
       </c>
       <c r="D219" s="2" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.2">
@@ -6728,9 +6734,9 @@
         <v>439</v>
       </c>
       <c r="D220" s="2" t="s">
-        <v>897</v>
-      </c>
-      <c r="E220" s="5" t="s">
+        <v>896</v>
+      </c>
+      <c r="E220" s="4" t="s">
         <v>787</v>
       </c>
     </row>
@@ -6745,7 +6751,7 @@
         <v>441</v>
       </c>
       <c r="D221" s="2" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.2">
@@ -6759,9 +6765,9 @@
         <v>443</v>
       </c>
       <c r="D222" s="2" t="s">
-        <v>899</v>
-      </c>
-      <c r="E222" s="5" t="s">
+        <v>898</v>
+      </c>
+      <c r="E222" s="4" t="s">
         <v>788</v>
       </c>
     </row>
@@ -6776,9 +6782,9 @@
         <v>445</v>
       </c>
       <c r="D223" s="2" t="s">
-        <v>900</v>
-      </c>
-      <c r="E223" s="5" t="s">
+        <v>899</v>
+      </c>
+      <c r="E223" s="4" t="s">
         <v>789</v>
       </c>
     </row>
@@ -6793,7 +6799,7 @@
         <v>447</v>
       </c>
       <c r="D224" s="2" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.2">
@@ -6807,7 +6813,7 @@
         <v>449</v>
       </c>
       <c r="D225" s="2" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.2">
@@ -6821,9 +6827,9 @@
         <v>451</v>
       </c>
       <c r="D226" s="2" t="s">
-        <v>903</v>
-      </c>
-      <c r="E226" s="5" t="s">
+        <v>902</v>
+      </c>
+      <c r="E226" s="4" t="s">
         <v>790</v>
       </c>
     </row>
@@ -6838,7 +6844,7 @@
         <v>453</v>
       </c>
       <c r="D227" s="2" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.2">
@@ -6852,7 +6858,7 @@
         <v>455</v>
       </c>
       <c r="D228" s="2" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.2">
@@ -6866,7 +6872,7 @@
         <v>457</v>
       </c>
       <c r="D229" s="2" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.2">
@@ -6880,7 +6886,7 @@
         <v>459</v>
       </c>
       <c r="D230" s="2" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.2">
@@ -6894,7 +6900,7 @@
         <v>461</v>
       </c>
       <c r="D231" s="2" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.2">
@@ -6908,7 +6914,7 @@
         <v>463</v>
       </c>
       <c r="D232" s="2" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.2">
@@ -6922,7 +6928,7 @@
         <v>465</v>
       </c>
       <c r="D233" s="2" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.2">
@@ -6936,7 +6942,7 @@
         <v>467</v>
       </c>
       <c r="D234" s="2" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.2">
@@ -6950,9 +6956,9 @@
         <v>469</v>
       </c>
       <c r="D235" s="2" t="s">
-        <v>908</v>
-      </c>
-      <c r="E235" s="5" t="s">
+        <v>907</v>
+      </c>
+      <c r="E235" s="4" t="s">
         <v>791</v>
       </c>
     </row>
@@ -6967,7 +6973,10 @@
         <v>471</v>
       </c>
       <c r="D236" s="2" t="s">
-        <v>913</v>
+        <v>912</v>
+      </c>
+      <c r="E236" s="4" t="s">
+        <v>792</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.2">
@@ -6981,7 +6990,10 @@
         <v>473</v>
       </c>
       <c r="D237" s="2" t="s">
-        <v>913</v>
+        <v>912</v>
+      </c>
+      <c r="E237" s="4" t="s">
+        <v>792</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.2">
@@ -6995,7 +7007,10 @@
         <v>475</v>
       </c>
       <c r="D238" s="2" t="s">
-        <v>913</v>
+        <v>912</v>
+      </c>
+      <c r="E238" s="4" t="s">
+        <v>792</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.2">
@@ -7009,9 +7024,9 @@
         <v>477</v>
       </c>
       <c r="D239" s="2" t="s">
-        <v>913</v>
-      </c>
-      <c r="E239" s="5" t="s">
+        <v>912</v>
+      </c>
+      <c r="E239" s="4" t="s">
         <v>792</v>
       </c>
     </row>
@@ -7025,7 +7040,7 @@
       <c r="C240" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="E240" s="5" t="s">
+      <c r="E240" s="4" t="s">
         <v>793</v>
       </c>
     </row>
@@ -7039,7 +7054,7 @@
       <c r="C241" s="2" t="s">
         <v>481</v>
       </c>
-      <c r="E241" s="5" t="s">
+      <c r="E241" s="4" t="s">
         <v>794</v>
       </c>
     </row>
@@ -7053,7 +7068,7 @@
       <c r="C242" s="2" t="s">
         <v>483</v>
       </c>
-      <c r="E242" s="5" t="s">
+      <c r="E242" s="4" t="s">
         <v>795</v>
       </c>
     </row>
@@ -7067,7 +7082,7 @@
       <c r="C243" s="2" t="s">
         <v>485</v>
       </c>
-      <c r="E243" s="5" t="s">
+      <c r="E243" s="4" t="s">
         <v>796</v>
       </c>
     </row>
@@ -7081,7 +7096,7 @@
       <c r="C244" s="2" t="s">
         <v>487</v>
       </c>
-      <c r="E244" s="5" t="s">
+      <c r="E244" s="4" t="s">
         <v>797</v>
       </c>
     </row>
@@ -7095,7 +7110,7 @@
       <c r="C245" s="2" t="s">
         <v>489</v>
       </c>
-      <c r="E245" s="5" t="s">
+      <c r="E245" s="4" t="s">
         <v>798</v>
       </c>
     </row>
@@ -7109,7 +7124,7 @@
       <c r="C246" s="2" t="s">
         <v>491</v>
       </c>
-      <c r="E246" s="5" t="s">
+      <c r="E246" s="4" t="s">
         <v>799</v>
       </c>
     </row>
@@ -7123,7 +7138,7 @@
       <c r="C247" s="2" t="s">
         <v>493</v>
       </c>
-      <c r="E247" s="5" t="s">
+      <c r="E247" s="4" t="s">
         <v>800</v>
       </c>
     </row>
@@ -7137,7 +7152,10 @@
       <c r="C248" s="2" t="s">
         <v>495</v>
       </c>
-      <c r="E248" s="5" t="s">
+      <c r="D248" t="s">
+        <v>916</v>
+      </c>
+      <c r="E248" s="4" t="s">
         <v>732</v>
       </c>
     </row>
@@ -7151,7 +7169,7 @@
       <c r="C249" s="2" t="s">
         <v>497</v>
       </c>
-      <c r="E249" s="5" t="s">
+      <c r="E249" s="4" t="s">
         <v>801</v>
       </c>
     </row>
@@ -7165,8 +7183,8 @@
       <c r="C250" s="2" t="s">
         <v>499</v>
       </c>
-      <c r="E250" s="5" t="s">
-        <v>802</v>
+      <c r="E250" s="4" t="s">
+        <v>917</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.2">
@@ -7179,8 +7197,8 @@
       <c r="C251" s="2" t="s">
         <v>501</v>
       </c>
-      <c r="E251" s="5" t="s">
-        <v>802</v>
+      <c r="E251" s="4" t="s">
+        <v>918</v>
       </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.2">
@@ -7193,8 +7211,8 @@
       <c r="C252" s="2" t="s">
         <v>503</v>
       </c>
-      <c r="E252" s="5" t="s">
-        <v>914</v>
+      <c r="E252" s="4" t="s">
+        <v>913</v>
       </c>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.2">
@@ -7207,8 +7225,8 @@
       <c r="C253" s="2" t="s">
         <v>505</v>
       </c>
-      <c r="E253" s="5" t="s">
-        <v>915</v>
+      <c r="E253" s="4" t="s">
+        <v>914</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.2">
@@ -7221,7 +7239,7 @@
       <c r="C254" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="E254" s="5" t="s">
+      <c r="E254" s="4" t="s">
         <v>729</v>
       </c>
     </row>
@@ -7235,7 +7253,7 @@
       <c r="C255" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="E255" s="5" t="s">
+      <c r="E255" s="4" t="s">
         <v>804</v>
       </c>
     </row>
@@ -7249,8 +7267,8 @@
       <c r="C256" s="2" t="s">
         <v>511</v>
       </c>
-      <c r="E256" s="5" t="s">
-        <v>916</v>
+      <c r="E256" s="4" t="s">
+        <v>915</v>
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.2">
@@ -7263,408 +7281,1601 @@
       <c r="C257" s="2" t="s">
         <v>513</v>
       </c>
-      <c r="E257" s="5" t="s">
+      <c r="E257" s="4" t="s">
         <v>806</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E258" s="5" t="s">
+      <c r="B258" s="2">
+        <v>256</v>
+      </c>
+      <c r="E258" s="4" t="s">
         <v>807</v>
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E259" s="5" t="s">
+      <c r="B259" s="2">
+        <v>257</v>
+      </c>
+      <c r="E259" s="4" t="s">
         <v>808</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E260" s="5" t="s">
+      <c r="B260" s="2">
+        <v>258</v>
+      </c>
+      <c r="E260" s="4" t="s">
         <v>809</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E261" s="5" t="s">
+      <c r="B261" s="2">
+        <v>259</v>
+      </c>
+      <c r="E261" s="4" t="s">
         <v>810</v>
       </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E262" s="5" t="s">
+      <c r="B262" s="2">
+        <v>260</v>
+      </c>
+      <c r="E262" s="4" t="s">
         <v>811</v>
       </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E263" s="5" t="s">
+      <c r="B263" s="2">
+        <v>261</v>
+      </c>
+      <c r="E263" s="4" t="s">
         <v>812</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E264" s="5" t="s">
+      <c r="B264" s="2">
+        <v>262</v>
+      </c>
+      <c r="E264" s="4" t="s">
         <v>813</v>
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E265" s="5" t="s">
+      <c r="B265" s="2">
+        <v>263</v>
+      </c>
+      <c r="E265" s="4" t="s">
         <v>814</v>
       </c>
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E266" s="5" t="s">
+      <c r="B266" s="2">
+        <v>264</v>
+      </c>
+      <c r="E266" s="4" t="s">
         <v>815</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E267" s="5" t="s">
+      <c r="B267" s="2">
+        <v>265</v>
+      </c>
+      <c r="E267" s="4" t="s">
         <v>816</v>
       </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E268" s="5" t="s">
+      <c r="B268" s="2">
+        <v>266</v>
+      </c>
+      <c r="E268" s="4" t="s">
         <v>817</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E269" s="5" t="s">
+      <c r="B269" s="2">
+        <v>267</v>
+      </c>
+      <c r="E269" s="4" t="s">
         <v>818</v>
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E270" s="5" t="s">
+      <c r="B270" s="2">
+        <v>268</v>
+      </c>
+      <c r="E270" s="4" t="s">
         <v>819</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E271" s="5" t="s">
+      <c r="B271" s="2">
+        <v>269</v>
+      </c>
+      <c r="E271" s="4" t="s">
         <v>820</v>
       </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E272" s="5" t="s">
+      <c r="B272" s="2">
+        <v>270</v>
+      </c>
+      <c r="E272" s="4" t="s">
         <v>821</v>
       </c>
     </row>
-    <row r="273" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E273" s="5" t="s">
+    <row r="273" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B273" s="2">
+        <v>271</v>
+      </c>
+      <c r="E273" s="4" t="s">
         <v>805</v>
       </c>
     </row>
-    <row r="274" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E274" s="5" t="s">
+    <row r="274" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B274" s="2">
+        <v>272</v>
+      </c>
+      <c r="E274" s="4" t="s">
         <v>784</v>
       </c>
     </row>
-    <row r="275" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E275" s="5" t="s">
+    <row r="275" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B275" s="2">
+        <v>273</v>
+      </c>
+      <c r="E275" s="4" t="s">
         <v>822</v>
       </c>
     </row>
-    <row r="276" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E276" s="5" t="s">
+    <row r="276" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B276" s="2">
+        <v>274</v>
+      </c>
+      <c r="E276" s="4" t="s">
         <v>823</v>
       </c>
     </row>
-    <row r="277" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E277" s="5" t="s">
+    <row r="277" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B277" s="2">
+        <v>275</v>
+      </c>
+      <c r="E277" s="4" t="s">
         <v>824</v>
       </c>
     </row>
-    <row r="278" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E278" s="5" t="s">
+    <row r="278" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B278" s="2">
+        <v>276</v>
+      </c>
+      <c r="E278" s="4" t="s">
         <v>805</v>
       </c>
     </row>
-    <row r="279" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E279" s="5" t="s">
+    <row r="279" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B279" s="2">
+        <v>277</v>
+      </c>
+      <c r="E279" s="4" t="s">
         <v>825</v>
       </c>
     </row>
-    <row r="280" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E280" s="5" t="s">
+    <row r="280" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B280" s="2">
+        <v>278</v>
+      </c>
+      <c r="E280" s="4" t="s">
         <v>826</v>
       </c>
     </row>
-    <row r="281" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E281" s="5" t="s">
+    <row r="281" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B281" s="2">
+        <v>279</v>
+      </c>
+      <c r="E281" s="4" t="s">
         <v>827</v>
       </c>
     </row>
-    <row r="282" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E282" s="5" t="s">
+    <row r="282" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B282" s="2">
+        <v>280</v>
+      </c>
+      <c r="E282" s="4" t="s">
         <v>826</v>
       </c>
     </row>
-    <row r="283" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E283" s="5" t="s">
+    <row r="283" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B283" s="2">
+        <v>281</v>
+      </c>
+      <c r="E283" s="4" t="s">
         <v>828</v>
       </c>
     </row>
-    <row r="284" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E284" s="5" t="s">
+    <row r="284" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B284" s="2">
+        <v>282</v>
+      </c>
+      <c r="E284" s="4" t="s">
         <v>829</v>
       </c>
     </row>
-    <row r="285" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E285" s="5" t="s">
+    <row r="285" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B285" s="2">
+        <v>283</v>
+      </c>
+      <c r="E285" s="4" t="s">
         <v>830</v>
       </c>
     </row>
-    <row r="286" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E286" s="5" t="s">
+    <row r="286" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B286" s="2">
+        <v>284</v>
+      </c>
+      <c r="E286" s="4" t="s">
         <v>831</v>
       </c>
     </row>
-    <row r="287" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E287" s="5" t="s">
+    <row r="287" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B287" s="2">
+        <v>285</v>
+      </c>
+      <c r="E287" s="4" t="s">
         <v>832</v>
       </c>
     </row>
-    <row r="288" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E288" s="5" t="s">
+    <row r="288" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B288" s="2">
+        <v>286</v>
+      </c>
+      <c r="E288" s="4" t="s">
         <v>833</v>
       </c>
     </row>
-    <row r="289" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E289" s="5" t="s">
+    <row r="289" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B289" s="2">
+        <v>287</v>
+      </c>
+      <c r="E289" s="4" t="s">
         <v>834</v>
       </c>
     </row>
-    <row r="290" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E290" s="5" t="s">
+    <row r="290" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B290" s="2">
+        <v>288</v>
+      </c>
+      <c r="E290" s="4" t="s">
         <v>835</v>
       </c>
     </row>
-    <row r="291" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E291" s="5" t="s">
+    <row r="291" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B291" s="2">
+        <v>289</v>
+      </c>
+      <c r="E291" s="4" t="s">
         <v>836</v>
       </c>
     </row>
-    <row r="292" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E292" s="5" t="s">
+    <row r="292" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B292" s="2">
+        <v>290</v>
+      </c>
+      <c r="E292" s="4" t="s">
         <v>831</v>
       </c>
     </row>
-    <row r="293" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E293" s="5" t="s">
+    <row r="293" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B293" s="2">
+        <v>291</v>
+      </c>
+      <c r="E293" s="4" t="s">
         <v>837</v>
       </c>
     </row>
-    <row r="294" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E294" s="5" t="s">
+    <row r="294" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B294" s="2">
+        <v>292</v>
+      </c>
+      <c r="E294" s="4" t="s">
         <v>838</v>
       </c>
     </row>
-    <row r="295" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E295" s="5" t="s">
+    <row r="295" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B295" s="2">
+        <v>293</v>
+      </c>
+      <c r="E295" s="4" t="s">
         <v>839</v>
       </c>
     </row>
-    <row r="296" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E296" s="5" t="s">
+    <row r="296" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B296" s="2">
+        <v>294</v>
+      </c>
+      <c r="E296" s="4" t="s">
         <v>840</v>
       </c>
     </row>
-    <row r="297" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E297" s="5" t="s">
+    <row r="297" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B297" s="2">
+        <v>295</v>
+      </c>
+      <c r="E297" s="4" t="s">
         <v>805</v>
       </c>
     </row>
-    <row r="298" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E298" s="5" t="s">
+    <row r="298" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B298" s="2">
+        <v>296</v>
+      </c>
+      <c r="E298" s="4" t="s">
         <v>841</v>
       </c>
     </row>
-    <row r="299" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E299" s="5" t="s">
+    <row r="299" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B299" s="2">
+        <v>297</v>
+      </c>
+      <c r="E299" s="4" t="s">
         <v>805</v>
       </c>
     </row>
-    <row r="300" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E300" s="5" t="s">
+    <row r="300" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B300" s="2">
+        <v>298</v>
+      </c>
+      <c r="E300" s="4" t="s">
         <v>842</v>
       </c>
     </row>
-    <row r="301" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E301" s="5" t="s">
+    <row r="301" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B301" s="2">
+        <v>299</v>
+      </c>
+      <c r="E301" s="4" t="s">
         <v>843</v>
       </c>
     </row>
-    <row r="302" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E302" s="5" t="s">
+    <row r="302" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B302" s="2">
+        <v>300</v>
+      </c>
+      <c r="E302" s="4" t="s">
         <v>844</v>
       </c>
     </row>
-    <row r="303" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E303" s="5" t="s">
+    <row r="303" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B303" s="2">
+        <v>301</v>
+      </c>
+      <c r="E303" s="4" t="s">
         <v>845</v>
       </c>
     </row>
-    <row r="304" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E304" s="5" t="s">
+    <row r="304" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B304" s="2">
+        <v>302</v>
+      </c>
+      <c r="E304" s="4" t="s">
         <v>846</v>
       </c>
     </row>
-    <row r="305" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E305" s="5" t="s">
+    <row r="305" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B305" s="2">
+        <v>303</v>
+      </c>
+      <c r="E305" s="4" t="s">
         <v>847</v>
       </c>
     </row>
-    <row r="306" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E306" s="5" t="s">
+    <row r="306" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B306" s="2">
+        <v>304</v>
+      </c>
+      <c r="E306" s="4" t="s">
         <v>848</v>
       </c>
     </row>
-    <row r="307" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E307" s="5" t="s">
+    <row r="307" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B307" s="2">
+        <v>305</v>
+      </c>
+      <c r="E307" s="4" t="s">
         <v>849</v>
       </c>
     </row>
-    <row r="308" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E308" s="5" t="s">
+    <row r="308" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B308" s="2">
+        <v>306</v>
+      </c>
+      <c r="E308" s="4" t="s">
         <v>850</v>
       </c>
     </row>
-    <row r="309" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E309" s="5" t="s">
+    <row r="309" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B309" s="2">
+        <v>307</v>
+      </c>
+      <c r="E309" s="4" t="s">
         <v>851</v>
       </c>
     </row>
-    <row r="310" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E310" s="5" t="s">
+    <row r="310" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B310" s="2">
+        <v>308</v>
+      </c>
+      <c r="E310" s="4" t="s">
         <v>852</v>
       </c>
     </row>
-    <row r="311" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E311" s="5" t="s">
+    <row r="311" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B311" s="2">
+        <v>309</v>
+      </c>
+      <c r="E311" s="4" t="s">
         <v>853</v>
       </c>
     </row>
-    <row r="312" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E312" s="5" t="s">
+    <row r="312" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B312" s="2">
+        <v>310</v>
+      </c>
+      <c r="E312" s="4" t="s">
         <v>854</v>
       </c>
     </row>
-    <row r="313" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E313" s="5" t="s">
+    <row r="313" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B313" s="2">
+        <v>311</v>
+      </c>
+      <c r="E313" s="4" t="s">
         <v>855</v>
       </c>
     </row>
-    <row r="314" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E314" s="5" t="s">
+    <row r="314" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B314" s="2">
+        <v>312</v>
+      </c>
+      <c r="E314" s="4" t="s">
         <v>856</v>
       </c>
     </row>
-    <row r="315" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E315" s="5" t="s">
+    <row r="315" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B315" s="2">
+        <v>313</v>
+      </c>
+      <c r="E315" s="4" t="s">
         <v>857</v>
       </c>
     </row>
-    <row r="316" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E316" s="5" t="s">
+    <row r="316" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B316" s="2">
+        <v>314</v>
+      </c>
+      <c r="E316" s="4" t="s">
         <v>858</v>
       </c>
     </row>
-    <row r="317" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E317" s="5" t="s">
+    <row r="317" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B317" s="2">
+        <v>315</v>
+      </c>
+      <c r="E317" s="4" t="s">
         <v>716</v>
       </c>
     </row>
-    <row r="318" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E318" s="5" t="s">
+    <row r="318" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B318" s="2">
+        <v>316</v>
+      </c>
+      <c r="E318" s="4" t="s">
         <v>859</v>
       </c>
     </row>
-    <row r="319" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E319" s="5" t="s">
+    <row r="319" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B319" s="2">
+        <v>317</v>
+      </c>
+      <c r="E319" s="4" t="s">
         <v>860</v>
       </c>
     </row>
-    <row r="320" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E320" s="5" t="s">
+    <row r="320" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B320" s="2">
+        <v>318</v>
+      </c>
+      <c r="E320" s="4" t="s">
         <v>861</v>
       </c>
     </row>
-    <row r="321" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E321" s="5" t="s">
+    <row r="321" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B321" s="2">
+        <v>319</v>
+      </c>
+      <c r="E321" s="4" t="s">
         <v>862</v>
       </c>
     </row>
-    <row r="322" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E322" s="5" t="s">
+    <row r="322" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B322" s="2">
+        <v>320</v>
+      </c>
+      <c r="E322" s="4" t="s">
         <v>863</v>
       </c>
     </row>
-    <row r="323" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E323" s="5" t="s">
+    <row r="323" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B323" s="2">
+        <v>321</v>
+      </c>
+      <c r="E323" s="4" t="s">
         <v>864</v>
       </c>
     </row>
-    <row r="324" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E324" s="5" t="s">
+    <row r="324" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B324" s="2">
+        <v>322</v>
+      </c>
+      <c r="E324" s="4" t="s">
         <v>865</v>
       </c>
     </row>
-    <row r="325" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E325" s="5" t="s">
+    <row r="325" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B325" s="2">
+        <v>323</v>
+      </c>
+      <c r="E325" s="4" t="s">
         <v>866</v>
       </c>
     </row>
-    <row r="326" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E326" s="5" t="s">
+    <row r="326" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B326" s="2">
+        <v>324</v>
+      </c>
+      <c r="E326" s="4" t="s">
         <v>867</v>
       </c>
     </row>
-    <row r="327" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E327" s="5" t="s">
+    <row r="327" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B327" s="2">
+        <v>325</v>
+      </c>
+      <c r="E327" s="4" t="s">
         <v>868</v>
       </c>
     </row>
-    <row r="328" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E328" s="5" t="s">
+    <row r="328" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B328" s="2">
+        <v>326</v>
+      </c>
+      <c r="E328" s="4" t="s">
         <v>869</v>
       </c>
     </row>
-    <row r="329" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E329" s="5" t="s">
+    <row r="329" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B329" s="2">
+        <v>327</v>
+      </c>
+      <c r="E329" s="4" t="s">
         <v>870</v>
       </c>
     </row>
-    <row r="330" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E330" s="5" t="s">
+    <row r="330" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B330" s="2">
+        <v>328</v>
+      </c>
+      <c r="E330" s="4" t="s">
         <v>871</v>
       </c>
     </row>
-    <row r="331" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E331" s="5" t="s">
+    <row r="331" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B331" s="2">
+        <v>329</v>
+      </c>
+      <c r="E331" s="4" t="s">
         <v>872</v>
       </c>
     </row>
-    <row r="332" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E332" s="5" t="s">
+    <row r="332" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B332" s="2">
+        <v>330</v>
+      </c>
+      <c r="E332" s="4" t="s">
         <v>873</v>
       </c>
     </row>
-    <row r="333" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E333" s="5" t="s">
+    <row r="333" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B333" s="2">
+        <v>331</v>
+      </c>
+      <c r="E333" s="4" t="s">
         <v>874</v>
       </c>
     </row>
-    <row r="334" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E334" s="5" t="s">
+    <row r="334" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B334" s="2">
+        <v>332</v>
+      </c>
+      <c r="E334" s="4" t="s">
         <v>875</v>
       </c>
     </row>
-    <row r="335" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E335" s="5" t="s">
+    <row r="335" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B335" s="2">
+        <v>333</v>
+      </c>
+      <c r="E335" s="4"/>
+    </row>
+    <row r="336" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B336" s="2">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="337" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B337" s="2">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="338" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B338" s="2">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="339" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B339" s="2">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="340" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B340" s="2">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="341" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B341" s="2">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="342" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B342" s="2">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="343" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B343" s="2">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="344" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B344" s="2">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="345" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B345" s="2">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="346" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B346" s="2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="347" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B347" s="2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="348" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B348" s="2">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="349" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B349" s="2">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="350" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B350" s="2">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="351" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B351" s="2">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="352" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B352" s="2">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="353" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B353" s="2">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="354" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B354" s="2">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="355" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B355" s="2">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="356" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B356" s="2">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="357" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B357" s="2">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="358" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B358" s="2">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="359" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B359" s="2">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="360" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B360" s="2">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="361" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B361" s="2">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="362" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B362" s="2">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="363" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B363" s="2">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="364" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B364" s="2">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="365" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B365" s="2">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="366" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B366" s="2">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="367" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B367" s="2">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="368" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B368" s="2">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="369" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B369" s="2">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="370" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B370" s="2">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="371" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B371" s="2">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="372" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B372" s="2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="373" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B373" s="2">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="374" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B374" s="2">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="375" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B375" s="2">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="376" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B376" s="2">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="377" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B377" s="2">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="378" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B378" s="2">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="379" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B379" s="2">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="380" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B380" s="2">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="381" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B381" s="2">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="382" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B382" s="2">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="383" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B383" s="2">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="384" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B384" s="2">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="385" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B385" s="2">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="386" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B386" s="2">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="387" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B387" s="2">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="388" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B388" s="2">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="389" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B389" s="2">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="390" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B390" s="2">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="391" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B391" s="2">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="392" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B392" s="2">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="393" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B393" s="2">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="394" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B394" s="2">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="395" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B395" s="2">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="396" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B396" s="2">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="397" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B397" s="2">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="398" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B398" s="2">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="399" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B399" s="2">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="400" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B400" s="2">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="401" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B401" s="2">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="402" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B402" s="2">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="403" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B403" s="2">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="404" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B404" s="2">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="405" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B405" s="2">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="406" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B406" s="2">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="407" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B407" s="2">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="408" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B408" s="2">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="409" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B409" s="2">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="410" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B410" s="2">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="411" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B411" s="2">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="412" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B412" s="2">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="413" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B413" s="2">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="414" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B414" s="2">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="415" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B415" s="2">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="416" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B416" s="2">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="417" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B417" s="2">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="418" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B418" s="2">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="419" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B419" s="2">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="420" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B420" s="2">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="421" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B421" s="2">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="422" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B422" s="2">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="423" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B423" s="2">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="424" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B424" s="2">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="425" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B425" s="2">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="426" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B426" s="2">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="427" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B427" s="2">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="428" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B428" s="2">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="429" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B429" s="2">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="430" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B430" s="2">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="431" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B431" s="2">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="432" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B432" s="2">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="433" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B433" s="2">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="434" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B434" s="2">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="435" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B435" s="2">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="436" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B436" s="2">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="437" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B437" s="2">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="438" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B438" s="2">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="439" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B439" s="2">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="440" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B440" s="2">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="441" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B441" s="2">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="442" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B442" s="2">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="443" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B443" s="2">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="444" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B444" s="2">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="445" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B445" s="2">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="446" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B446" s="2">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="447" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B447" s="2">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="448" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B448" s="2">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="449" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B449" s="2">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="450" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B450" s="2">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="451" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B451" s="2">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="452" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B452" s="2">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="453" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B453" s="2">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="454" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B454" s="2">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="455" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B455" s="2">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="456" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B456" s="2">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="457" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B457" s="2">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="458" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B458" s="2">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="459" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B459" s="2">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="460" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B460" s="2">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="461" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B461" s="2">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="462" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B462" s="2">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="463" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B463" s="2">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="464" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B464" s="2">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="465" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B465" s="2">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="466" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B466" s="2">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="467" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B467" s="2">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="468" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B468" s="2">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="469" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B469" s="2">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="470" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B470" s="2">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="471" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B471" s="2">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="472" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B472" s="2">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="473" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B473" s="2">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="474" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B474" s="2">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="475" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B475" s="2">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="476" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B476" s="2">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="477" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B477" s="2">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="478" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B478" s="2">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="479" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B479" s="2">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="480" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B480" s="2">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="481" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B481" s="2">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="482" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B482" s="2">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="483" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B483" s="2">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="484" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B484" s="2">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="485" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B485" s="2">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="486" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B486" s="2">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="487" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B487" s="2">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="488" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B488" s="2">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="489" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B489" s="2">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="490" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B490" s="2">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="491" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B491" s="2">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="492" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B492" s="2">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="493" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B493" s="2">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="494" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B494" s="2">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="495" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B495" s="2">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="496" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B496" s="2">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="497" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B497" s="2">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="498" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B498" s="2">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="499" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B499" s="2">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="500" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B500" s="2">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="501" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B501" s="2">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="502" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B502" s="2">
+        <v>500</v>
+      </c>
+      <c r="E502" s="4" t="s">
         <v>876</v>
       </c>
     </row>
-    <row r="336" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E336" s="5" t="s">
+    <row r="503" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B503" s="2">
+        <v>501</v>
+      </c>
+      <c r="E503" s="4" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="504" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B504" s="2">
+        <v>502</v>
+      </c>
+      <c r="E504" s="4" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="505" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B505" s="2">
+        <v>503</v>
+      </c>
+      <c r="E505" s="4" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="506" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B506" s="2">
+        <v>504</v>
+      </c>
+      <c r="E506" s="4" t="s">
         <v>877</v>
       </c>
     </row>
-    <row r="337" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E337" s="5" t="s">
+    <row r="507" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B507" s="2">
+        <v>505</v>
+      </c>
+      <c r="E507" s="4" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="508" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B508" s="2">
+        <v>506</v>
+      </c>
+      <c r="E508" s="4" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="509" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B509" s="2">
+        <v>507</v>
+      </c>
+      <c r="E509" s="4" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="510" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B510" s="2">
+        <v>508</v>
+      </c>
+      <c r="E510" s="4" t="s">
         <v>878</v>
+      </c>
+    </row>
+    <row r="511" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B511" s="2">
+        <v>509</v>
+      </c>
+      <c r="E511" s="4" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="512" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B512" s="2">
+        <v>510</v>
+      </c>
+      <c r="E512" s="4" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="513" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B513" s="2">
+        <v>511</v>
+      </c>
+      <c r="E513" s="4" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="514" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B514" s="2">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="515" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B515" s="2">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="516" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B516" s="2">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="517" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B517" s="2">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="518" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B518" s="2">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="519" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B519" s="2">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="520" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B520" s="2">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="521" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B521" s="2">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="522" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B522" s="2">
+        <v>520</v>
       </c>
     </row>
   </sheetData>
@@ -7684,1077 +8895,1077 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>682</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>683</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>684</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>685</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>686</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>687</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>688</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>687</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>689</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>690</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>691</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>692</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>693</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>694</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>695</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>696</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>697</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>698</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>699</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>700</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
         <v>701</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="3" t="s">
         <v>702</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="3" t="s">
         <v>703</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="3" t="s">
         <v>704</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="3" t="s">
         <v>705</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="3" t="s">
         <v>706</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="3" t="s">
         <v>707</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="3" t="s">
         <v>708</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="3" t="s">
         <v>709</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="3" t="s">
         <v>710</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="3" t="s">
         <v>711</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="3" t="s">
         <v>712</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="3" t="s">
         <v>713</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="3" t="s">
         <v>714</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="3" t="s">
         <v>715</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="3" t="s">
         <v>716</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="3" t="s">
         <v>717</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="3" t="s">
         <v>718</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="3" t="s">
         <v>719</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="3" t="s">
         <v>720</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="3" t="s">
         <v>721</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="3" t="s">
         <v>722</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="3" t="s">
         <v>723</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="3" t="s">
         <v>724</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" s="4" t="s">
+      <c r="A45" s="3" t="s">
         <v>725</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="3" t="s">
         <v>726</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="3" t="s">
         <v>727</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" s="4" t="s">
+      <c r="A48" s="3" t="s">
         <v>728</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="4" t="s">
+      <c r="A49" s="3" t="s">
         <v>729</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" s="4" t="s">
+      <c r="A50" s="3" t="s">
         <v>730</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="3" t="s">
         <v>731</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" s="4" t="s">
+      <c r="A52" s="3" t="s">
         <v>732</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" s="4" t="s">
+      <c r="A53" s="3" t="s">
         <v>733</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" s="4" t="s">
+      <c r="A54" s="3" t="s">
         <v>734</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" s="4" t="s">
+      <c r="A55" s="3" t="s">
         <v>735</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" s="4" t="s">
+      <c r="A56" s="3" t="s">
         <v>736</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" s="4" t="s">
+      <c r="A57" s="3" t="s">
         <v>737</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" s="4" t="s">
+      <c r="A58" s="3" t="s">
         <v>737</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A59" s="4" t="s">
+      <c r="A59" s="3" t="s">
         <v>738</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A60" s="4" t="s">
+      <c r="A60" s="3" t="s">
         <v>739</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A61" s="4" t="s">
+      <c r="A61" s="3" t="s">
         <v>740</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62" s="4" t="s">
+      <c r="A62" s="3" t="s">
         <v>741</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A63" s="4" t="s">
+      <c r="A63" s="3" t="s">
         <v>742</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64" s="4" t="s">
+      <c r="A64" s="3" t="s">
         <v>743</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" s="4" t="s">
+      <c r="A65" s="3" t="s">
         <v>744</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" s="4" t="s">
+      <c r="A66" s="3" t="s">
         <v>732</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67" s="4" t="s">
+      <c r="A67" s="3" t="s">
         <v>745</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A68" s="4" t="s">
+      <c r="A68" s="3" t="s">
         <v>746</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A69" s="4" t="s">
+      <c r="A69" s="3" t="s">
         <v>747</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A70" s="4" t="s">
+      <c r="A70" s="3" t="s">
         <v>748</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71" s="4" t="s">
+      <c r="A71" s="3" t="s">
         <v>749</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A72" s="4" t="s">
+      <c r="A72" s="3" t="s">
         <v>750</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A73" s="4" t="s">
+      <c r="A73" s="3" t="s">
         <v>751</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A74" s="4" t="s">
+      <c r="A74" s="3" t="s">
         <v>752</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A75" s="4" t="s">
+      <c r="A75" s="3" t="s">
         <v>753</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A76" s="4" t="s">
+      <c r="A76" s="3" t="s">
         <v>754</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A77" s="4" t="s">
+      <c r="A77" s="3" t="s">
         <v>755</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A78" s="4" t="s">
+      <c r="A78" s="3" t="s">
         <v>756</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A79" s="4" t="s">
+      <c r="A79" s="3" t="s">
         <v>757</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A80" s="4" t="s">
+      <c r="A80" s="3" t="s">
         <v>732</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A81" s="4" t="s">
+      <c r="A81" s="3" t="s">
         <v>758</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A82" s="4" t="s">
+      <c r="A82" s="3" t="s">
         <v>759</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A83" s="4" t="s">
+      <c r="A83" s="3" t="s">
         <v>760</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A84" s="4" t="s">
+      <c r="A84" s="3" t="s">
         <v>732</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A85" s="4" t="s">
+      <c r="A85" s="3" t="s">
         <v>761</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A86" s="4" t="s">
+      <c r="A86" s="3" t="s">
         <v>762</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A87" s="4" t="s">
+      <c r="A87" s="3" t="s">
         <v>763</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A88" s="4" t="s">
+      <c r="A88" s="3" t="s">
         <v>764</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A89" s="4" t="s">
+      <c r="A89" s="3" t="s">
         <v>765</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A90" s="4" t="s">
+      <c r="A90" s="3" t="s">
         <v>766</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A91" s="4" t="s">
+      <c r="A91" s="3" t="s">
         <v>767</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A92" s="4" t="s">
+      <c r="A92" s="3" t="s">
         <v>768</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A93" s="4" t="s">
+      <c r="A93" s="3" t="s">
         <v>769</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A94" s="4" t="s">
+      <c r="A94" s="3" t="s">
         <v>770</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A95" s="4" t="s">
+      <c r="A95" s="3" t="s">
         <v>771</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A96" s="4" t="s">
+      <c r="A96" s="3" t="s">
         <v>772</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A97" s="4" t="s">
+      <c r="A97" s="3" t="s">
         <v>773</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A98" s="4" t="s">
+      <c r="A98" s="3" t="s">
         <v>774</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A99" s="4" t="s">
+      <c r="A99" s="3" t="s">
         <v>775</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A100" s="4" t="s">
+      <c r="A100" s="3" t="s">
         <v>776</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A101" s="4" t="s">
+      <c r="A101" s="3" t="s">
         <v>777</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A102" s="4" t="s">
+      <c r="A102" s="3" t="s">
         <v>778</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A103" s="4" t="s">
+      <c r="A103" s="3" t="s">
         <v>779</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A104" s="4" t="s">
+      <c r="A104" s="3" t="s">
         <v>780</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A105" s="4" t="s">
+      <c r="A105" s="3" t="s">
         <v>781</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A106" s="4" t="s">
+      <c r="A106" s="3" t="s">
         <v>782</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A107" s="4" t="s">
+      <c r="A107" s="3" t="s">
         <v>732</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A108" s="4" t="s">
+      <c r="A108" s="3" t="s">
         <v>783</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A109" s="4" t="s">
+      <c r="A109" s="3" t="s">
         <v>784</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A110" s="4" t="s">
+      <c r="A110" s="3" t="s">
         <v>785</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A111" s="4" t="s">
+      <c r="A111" s="3" t="s">
         <v>732</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A112" s="4" t="s">
+      <c r="A112" s="3" t="s">
         <v>786</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A113" s="4" t="s">
+      <c r="A113" s="3" t="s">
         <v>732</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A114" s="4" t="s">
+      <c r="A114" s="3" t="s">
         <v>787</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A115" s="4" t="s">
+      <c r="A115" s="3" t="s">
         <v>788</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A116" s="4" t="s">
+      <c r="A116" s="3" t="s">
         <v>789</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A117" s="4" t="s">
+      <c r="A117" s="3" t="s">
         <v>790</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A118" s="4" t="s">
+      <c r="A118" s="3" t="s">
         <v>791</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A119" s="4" t="s">
+      <c r="A119" s="3" t="s">
         <v>792</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A120" s="4" t="s">
+      <c r="A120" s="3" t="s">
         <v>793</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A121" s="4" t="s">
+      <c r="A121" s="3" t="s">
         <v>794</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A122" s="4" t="s">
+      <c r="A122" s="3" t="s">
         <v>795</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A123" s="4" t="s">
+      <c r="A123" s="3" t="s">
         <v>796</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A124" s="4" t="s">
+      <c r="A124" s="3" t="s">
         <v>797</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A125" s="4" t="s">
+      <c r="A125" s="3" t="s">
         <v>798</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A126" s="4" t="s">
+      <c r="A126" s="3" t="s">
         <v>799</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A127" s="4" t="s">
+      <c r="A127" s="3" t="s">
         <v>800</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A128" s="4" t="s">
+      <c r="A128" s="3" t="s">
         <v>732</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A129" s="4" t="s">
+      <c r="A129" s="3" t="s">
         <v>801</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A130" s="4" t="s">
+      <c r="A130" s="3" t="s">
         <v>802</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A131" s="4" t="s">
+      <c r="A131" s="3" t="s">
         <v>803</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A132" s="4" t="s">
+      <c r="A132" s="3" t="s">
         <v>729</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A133" s="4" t="s">
+      <c r="A133" s="3" t="s">
         <v>804</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A134" s="4" t="s">
+      <c r="A134" s="3" t="s">
         <v>805</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A135" s="4" t="s">
+      <c r="A135" s="3" t="s">
         <v>806</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A136" s="4" t="s">
+      <c r="A136" s="3" t="s">
         <v>807</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A137" s="4" t="s">
+      <c r="A137" s="3" t="s">
         <v>808</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A138" s="4" t="s">
+      <c r="A138" s="3" t="s">
         <v>809</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A139" s="4" t="s">
+      <c r="A139" s="3" t="s">
         <v>810</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A140" s="4" t="s">
+      <c r="A140" s="3" t="s">
         <v>811</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A141" s="4" t="s">
+      <c r="A141" s="3" t="s">
         <v>812</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A142" s="4" t="s">
+      <c r="A142" s="3" t="s">
         <v>813</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A143" s="4" t="s">
+      <c r="A143" s="3" t="s">
         <v>814</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A144" s="4" t="s">
+      <c r="A144" s="3" t="s">
         <v>815</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A145" s="4" t="s">
+      <c r="A145" s="3" t="s">
         <v>816</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A146" s="4" t="s">
+      <c r="A146" s="3" t="s">
         <v>817</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A147" s="4" t="s">
+      <c r="A147" s="3" t="s">
         <v>818</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A148" s="4" t="s">
+      <c r="A148" s="3" t="s">
         <v>819</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A149" s="4" t="s">
+      <c r="A149" s="3" t="s">
         <v>820</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A150" s="4" t="s">
+      <c r="A150" s="3" t="s">
         <v>821</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A151" s="4" t="s">
+      <c r="A151" s="3" t="s">
         <v>805</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A152" s="4" t="s">
+      <c r="A152" s="3" t="s">
         <v>784</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A153" s="4" t="s">
+      <c r="A153" s="3" t="s">
         <v>822</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A154" s="4" t="s">
+      <c r="A154" s="3" t="s">
         <v>823</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A155" s="4" t="s">
+      <c r="A155" s="3" t="s">
         <v>824</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A156" s="4" t="s">
+      <c r="A156" s="3" t="s">
         <v>805</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A157" s="4" t="s">
+      <c r="A157" s="3" t="s">
         <v>825</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A158" s="4" t="s">
+      <c r="A158" s="3" t="s">
         <v>826</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A159" s="4" t="s">
+      <c r="A159" s="3" t="s">
         <v>827</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A160" s="4" t="s">
+      <c r="A160" s="3" t="s">
         <v>826</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A161" s="4" t="s">
+      <c r="A161" s="3" t="s">
         <v>828</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A162" s="4" t="s">
+      <c r="A162" s="3" t="s">
         <v>829</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A163" s="4" t="s">
+      <c r="A163" s="3" t="s">
         <v>830</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A164" s="4" t="s">
+      <c r="A164" s="3" t="s">
         <v>831</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A165" s="4" t="s">
+      <c r="A165" s="3" t="s">
         <v>832</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A166" s="4" t="s">
+      <c r="A166" s="3" t="s">
         <v>833</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A167" s="4" t="s">
+      <c r="A167" s="3" t="s">
         <v>834</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A168" s="4" t="s">
+      <c r="A168" s="3" t="s">
         <v>835</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A169" s="4" t="s">
+      <c r="A169" s="3" t="s">
         <v>836</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A170" s="4" t="s">
+      <c r="A170" s="3" t="s">
         <v>831</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A171" s="4" t="s">
+      <c r="A171" s="3" t="s">
         <v>837</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A172" s="4" t="s">
+      <c r="A172" s="3" t="s">
         <v>838</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A173" s="4" t="s">
+      <c r="A173" s="3" t="s">
         <v>839</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A174" s="4" t="s">
+      <c r="A174" s="3" t="s">
         <v>840</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A175" s="4" t="s">
+      <c r="A175" s="3" t="s">
         <v>805</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A176" s="4" t="s">
+      <c r="A176" s="3" t="s">
         <v>841</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A177" s="4" t="s">
+      <c r="A177" s="3" t="s">
         <v>805</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A178" s="4" t="s">
+      <c r="A178" s="3" t="s">
         <v>842</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A179" s="4" t="s">
+      <c r="A179" s="3" t="s">
         <v>843</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A180" s="4" t="s">
+      <c r="A180" s="3" t="s">
         <v>844</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A181" s="4" t="s">
+      <c r="A181" s="3" t="s">
         <v>845</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A182" s="4" t="s">
+      <c r="A182" s="3" t="s">
         <v>846</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A183" s="4" t="s">
+      <c r="A183" s="3" t="s">
         <v>847</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A184" s="4" t="s">
+      <c r="A184" s="3" t="s">
         <v>848</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A185" s="4" t="s">
+      <c r="A185" s="3" t="s">
         <v>849</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A186" s="4" t="s">
+      <c r="A186" s="3" t="s">
         <v>850</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A187" s="4" t="s">
+      <c r="A187" s="3" t="s">
         <v>851</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A188" s="4" t="s">
+      <c r="A188" s="3" t="s">
         <v>852</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A189" s="4" t="s">
+      <c r="A189" s="3" t="s">
         <v>853</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A190" s="4" t="s">
+      <c r="A190" s="3" t="s">
         <v>854</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A191" s="4" t="s">
+      <c r="A191" s="3" t="s">
         <v>855</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A192" s="4" t="s">
+      <c r="A192" s="3" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A193" s="4" t="s">
+      <c r="A193" s="3" t="s">
         <v>857</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A194" s="4" t="s">
+      <c r="A194" s="3" t="s">
         <v>858</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A195" s="4" t="s">
+      <c r="A195" s="3" t="s">
         <v>716</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A196" s="4" t="s">
+      <c r="A196" s="3" t="s">
         <v>859</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A197" s="4" t="s">
+      <c r="A197" s="3" t="s">
         <v>860</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A198" s="4" t="s">
+      <c r="A198" s="3" t="s">
         <v>861</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A199" s="4" t="s">
+      <c r="A199" s="3" t="s">
         <v>862</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A200" s="4" t="s">
+      <c r="A200" s="3" t="s">
         <v>863</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A201" s="4" t="s">
+      <c r="A201" s="3" t="s">
         <v>864</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A202" s="4" t="s">
+      <c r="A202" s="3" t="s">
         <v>865</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A203" s="4" t="s">
+      <c r="A203" s="3" t="s">
         <v>866</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A204" s="4" t="s">
+      <c r="A204" s="3" t="s">
         <v>867</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A205" s="4" t="s">
+      <c r="A205" s="3" t="s">
         <v>868</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A206" s="4" t="s">
+      <c r="A206" s="3" t="s">
         <v>869</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A207" s="4" t="s">
+      <c r="A207" s="3" t="s">
         <v>870</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A208" s="4" t="s">
+      <c r="A208" s="3" t="s">
         <v>871</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A209" s="4" t="s">
+      <c r="A209" s="3" t="s">
         <v>872</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A210" s="4" t="s">
+      <c r="A210" s="3" t="s">
         <v>873</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A211" s="4" t="s">
+      <c r="A211" s="3" t="s">
         <v>874</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A212" s="4" t="s">
+      <c r="A212" s="3" t="s">
         <v>875</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A213" s="4" t="s">
+      <c r="A213" s="3" t="s">
         <v>876</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A214" s="4" t="s">
+      <c r="A214" s="3" t="s">
         <v>877</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A215" s="4" t="s">
+      <c r="A215" s="3" t="s">
         <v>878</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add initial meta-prompt for reasoning models
</commit_message>
<xml_diff>
--- a/RPG/images/U4 and 5 Image data.xlsx
+++ b/RPG/images/U4 and 5 Image data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tedtschopp/Developer/tedt.org/RPG/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23F17E2-3A1A-4D42-9C58-41660B51FD22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{983C3E3E-3D42-6741-AF06-FBCA8CF4EE9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="620" windowWidth="25620" windowHeight="28180" xr2:uid="{899837AF-DA2E-EC45-BB45-3151DAABF807}"/>
+    <workbookView xWindow="17700" yWindow="900" windowWidth="25640" windowHeight="28180" xr2:uid="{899837AF-DA2E-EC45-BB45-3151DAABF807}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2905,16 +2905,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>698500</xdr:colOff>
-      <xdr:row>203</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>774700</xdr:colOff>
-      <xdr:row>235</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2944,7 +2944,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4508500" y="41440100"/>
+          <a:off x="9918700" y="139700"/>
           <a:ext cx="13004800" cy="6502400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3286,14 +3286,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C257557-0CE3-7C44-B9BE-3642D5280C90}">
   <dimension ref="A1:E522"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B196" workbookViewId="0">
-      <selection activeCell="D208" sqref="D208"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.83203125" customWidth="1"/>
+    <col min="5" max="5" width="50.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>